<commit_message>
add:api doc and fix:function
</commit_message>
<xml_diff>
--- a/docs/hidden_기능설계.xlsx
+++ b/docs/hidden_기능설계.xlsx
@@ -267,7 +267,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11.0"/>
       <name val="맑은 고딕"/>
@@ -386,15 +386,10 @@
     <font>
       <sz val="11.0"/>
       <name val="맑은 고딕"/>
-      <color rgb="FFFF0000"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <name val="맑은 고딕"/>
-      <color/>
+      <color rgb="FF000000"/>
     </font>
   </fonts>
-  <fills count="44">
+  <fills count="43">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -599,12 +594,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399980"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -691,7 +680,6 @@
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -700,7 +688,6 @@
       <bottom style="thick">
         <color theme="4"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -709,7 +696,6 @@
       <bottom style="thick">
         <color rgb="FFACCCEA"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -718,7 +704,6 @@
       <bottom style="medium">
         <color theme="4" tint="0.399980"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -733,7 +718,6 @@
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -748,7 +732,6 @@
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="double">
@@ -763,7 +746,6 @@
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -772,7 +754,6 @@
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -783,7 +764,6 @@
       <bottom style="double">
         <color theme="4"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
@@ -935,7 +915,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -960,23 +940,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="28" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="35" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="28" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -984,9 +973,6 @@
     <xf numFmtId="176" fontId="0" fillId="36" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -999,6 +985,9 @@
     <xf numFmtId="176" fontId="0" fillId="38" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="38" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1017,6 +1006,9 @@
     <xf numFmtId="0" fontId="4" fillId="40" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="41" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1026,47 +1018,38 @@
     <xf numFmtId="0" fontId="4" fillId="41" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="42" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="42" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="42" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="43" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="43" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="41" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="42" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="41" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="41" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="42" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="43" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="21" fillId="41" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="21" fillId="42" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="42" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="43" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="22" fillId="42" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="22" fillId="43" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1389,7 +1372,7 @@
   <dimension ref="B2:O52"/>
   <sheetViews>
     <sheetView topLeftCell="B1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.500000"/>
@@ -1809,60 +1792,60 @@
       <c r="O15" s="27"/>
     </row>
     <row r="16" spans="2:15">
-      <c r="B16" s="19">
+      <c r="B16" s="34">
         <v>14</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19" t="s">
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="L16" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="M16" s="20" t="s">
+      <c r="L16" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="M16" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="N16" s="19"/>
-      <c r="O16" s="19"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="34"/>
     </row>
     <row r="17" spans="2:15">
-      <c r="B17" s="19">
+      <c r="B17" s="34">
         <v>15</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19" t="s">
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19" t="s">
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="L17" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="M17" s="20" t="s">
+      <c r="L17" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="M17" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
     </row>
     <row r="18" spans="2:15">
       <c r="B18" s="14">
@@ -2131,30 +2114,30 @@
       <c r="O27" s="31"/>
     </row>
     <row r="28" spans="2:15">
-      <c r="B28" s="19">
+      <c r="B28" s="34">
         <v>26</v>
       </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="19" t="s">
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19" t="s">
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="34"/>
+      <c r="J28" s="34"/>
+      <c r="K28" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="L28" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="M28" s="20" t="s">
+      <c r="L28" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="M28" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="N28" s="19"/>
-      <c r="O28" s="19"/>
+      <c r="N28" s="34"/>
+      <c r="O28" s="34"/>
     </row>
     <row r="29" spans="2:15">
       <c r="B29" s="3"/>
@@ -2482,8 +2465,7 @@
     <col min="10" max="10" style="3" width="25.37999916" customWidth="1" outlineLevel="0"/>
     <col min="11" max="14" style="3" width="9.00500011" customWidth="1" outlineLevel="0"/>
     <col min="15" max="15" style="3" width="25.62999916" customWidth="1" outlineLevel="0"/>
-    <col min="16" max="16" style="3" width="9.00500011" customWidth="1" outlineLevel="0"/>
-    <col min="17" max="16384" style="3" width="9.00500011" customWidth="1" outlineLevel="0"/>
+    <col min="16" max="16384" style="3" width="9.00500011" customWidth="1" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15">

</xml_diff>